<commit_message>
Created a separate repo for My Kicad Library
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chipc\Documents\PCB\KiCAD_Repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chipc\Documents\PCB\KiCAD_REPOS\KClib_CBC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2088" windowHeight="7272" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2088" windowHeight="7272" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CAP" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated BOM with 1x12 Pin Header
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17429" uniqueCount="7847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17436" uniqueCount="7852">
   <si>
     <t>House Part Number</t>
   </si>
@@ -23571,6 +23571,21 @@
   </si>
   <si>
     <t>Plug - PTSM 0,5/ 8-P-2,5 WH</t>
+  </si>
+  <si>
+    <t>CON-1006-12</t>
+  </si>
+  <si>
+    <t>1x12</t>
+  </si>
+  <si>
+    <t>PRPC012SAAN-RC</t>
+  </si>
+  <si>
+    <t>Pin Header, Straight, 2.54mm pitch, 1x12, 0.025" SQ Pin</t>
+  </si>
+  <si>
+    <t>CBC_Connectors:Pin_Header_Straight_1x12_Pitch2.54mm</t>
   </si>
 </sst>
 </file>
@@ -78771,11 +78786,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -79667,42 +79682,42 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>7750</v>
+        <v>7847</v>
       </c>
       <c r="B43" t="s">
-        <v>7782</v>
+        <v>7848</v>
       </c>
       <c r="C43" t="s">
-        <v>7751</v>
-      </c>
-      <c r="D43">
-        <v>3568</v>
+        <v>7529</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7849</v>
       </c>
       <c r="E43" t="s">
-        <v>7761</v>
+        <v>7850</v>
       </c>
       <c r="F43" t="s">
         <v>6374</v>
       </c>
       <c r="G43" t="s">
-        <v>7752</v>
+        <v>7851</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>7753</v>
+        <v>7750</v>
       </c>
       <c r="B44" t="s">
-        <v>7773</v>
+        <v>7782</v>
       </c>
       <c r="C44" t="s">
         <v>7751</v>
       </c>
-      <c r="D44" t="s">
-        <v>7776</v>
+      <c r="D44">
+        <v>3568</v>
       </c>
       <c r="E44" t="s">
-        <v>7779</v>
+        <v>7761</v>
       </c>
       <c r="F44" t="s">
         <v>6374</v>
@@ -79713,19 +79728,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>7771</v>
+        <v>7753</v>
       </c>
       <c r="B45" t="s">
-        <v>7774</v>
+        <v>7773</v>
       </c>
       <c r="C45" t="s">
         <v>7751</v>
       </c>
       <c r="D45" t="s">
-        <v>7777</v>
+        <v>7776</v>
       </c>
       <c r="E45" t="s">
-        <v>7780</v>
+        <v>7779</v>
       </c>
       <c r="F45" t="s">
         <v>6374</v>
@@ -79736,19 +79751,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>7772</v>
+        <v>7771</v>
       </c>
       <c r="B46" t="s">
-        <v>7775</v>
+        <v>7774</v>
       </c>
       <c r="C46" t="s">
         <v>7751</v>
       </c>
       <c r="D46" t="s">
-        <v>7778</v>
+        <v>7777</v>
       </c>
       <c r="E46" t="s">
-        <v>7781</v>
+        <v>7780</v>
       </c>
       <c r="F46" t="s">
         <v>6374</v>
@@ -79759,42 +79774,42 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>7755</v>
+        <v>7772</v>
       </c>
       <c r="B47" t="s">
-        <v>7756</v>
+        <v>7775</v>
       </c>
       <c r="C47" t="s">
         <v>7751</v>
       </c>
       <c r="D47" t="s">
-        <v>7754</v>
+        <v>7778</v>
       </c>
       <c r="E47" t="s">
-        <v>7760</v>
+        <v>7781</v>
       </c>
       <c r="F47" t="s">
         <v>6374</v>
       </c>
       <c r="G47" t="s">
-        <v>7783</v>
+        <v>7752</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>7762</v>
+        <v>7755</v>
       </c>
       <c r="B48" t="s">
-        <v>7765</v>
+        <v>7756</v>
       </c>
       <c r="C48" t="s">
         <v>7751</v>
       </c>
       <c r="D48" t="s">
-        <v>7757</v>
+        <v>7754</v>
       </c>
       <c r="E48" t="s">
-        <v>7768</v>
+        <v>7760</v>
       </c>
       <c r="F48" t="s">
         <v>6374</v>
@@ -79805,19 +79820,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>7763</v>
+        <v>7762</v>
       </c>
       <c r="B49" t="s">
-        <v>7766</v>
+        <v>7765</v>
       </c>
       <c r="C49" t="s">
         <v>7751</v>
       </c>
       <c r="D49" t="s">
-        <v>7758</v>
+        <v>7757</v>
       </c>
       <c r="E49" t="s">
-        <v>7769</v>
+        <v>7768</v>
       </c>
       <c r="F49" t="s">
         <v>6374</v>
@@ -79828,19 +79843,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>7764</v>
+        <v>7763</v>
       </c>
       <c r="B50" t="s">
-        <v>7767</v>
+        <v>7766</v>
       </c>
       <c r="C50" t="s">
         <v>7751</v>
       </c>
       <c r="D50" t="s">
-        <v>7759</v>
+        <v>7758</v>
       </c>
       <c r="E50" t="s">
-        <v>7770</v>
+        <v>7769</v>
       </c>
       <c r="F50" t="s">
         <v>6374</v>
@@ -79851,88 +79866,88 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>7416</v>
+        <v>7764</v>
       </c>
       <c r="B51" t="s">
-        <v>7417</v>
+        <v>7767</v>
       </c>
       <c r="C51" t="s">
-        <v>7418</v>
+        <v>7751</v>
       </c>
       <c r="D51" t="s">
-        <v>7419</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>7420</v>
+        <v>7759</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7770</v>
       </c>
       <c r="F51" t="s">
-        <v>7713</v>
+        <v>6374</v>
       </c>
       <c r="G51" t="s">
-        <v>7422</v>
+        <v>7783</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>7629</v>
+        <v>7416</v>
       </c>
       <c r="B52" t="s">
-        <v>7682</v>
+        <v>7417</v>
       </c>
       <c r="C52" t="s">
-        <v>7626</v>
+        <v>7418</v>
       </c>
       <c r="D52" t="s">
-        <v>7625</v>
-      </c>
-      <c r="E52" t="s">
-        <v>7627</v>
+        <v>7419</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>7420</v>
       </c>
       <c r="F52" t="s">
         <v>7713</v>
       </c>
       <c r="G52" t="s">
-        <v>7628</v>
+        <v>7422</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>7637</v>
+        <v>7629</v>
       </c>
       <c r="B53" t="s">
-        <v>7683</v>
+        <v>7682</v>
       </c>
       <c r="C53" t="s">
-        <v>7660</v>
+        <v>7626</v>
       </c>
       <c r="D53" t="s">
-        <v>7636</v>
+        <v>7625</v>
       </c>
       <c r="E53" t="s">
-        <v>7650</v>
+        <v>7627</v>
       </c>
       <c r="F53" t="s">
         <v>7713</v>
       </c>
       <c r="G53" t="s">
-        <v>7661</v>
+        <v>7628</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>7638</v>
+        <v>7637</v>
       </c>
       <c r="B54" t="s">
-        <v>7684</v>
+        <v>7683</v>
       </c>
       <c r="C54" t="s">
         <v>7660</v>
       </c>
       <c r="D54" t="s">
-        <v>7644</v>
+        <v>7636</v>
       </c>
       <c r="E54" t="s">
-        <v>7651</v>
+        <v>7650</v>
       </c>
       <c r="F54" t="s">
         <v>7713</v>
@@ -79943,7 +79958,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>7819</v>
+        <v>7638</v>
       </c>
       <c r="B55" t="s">
         <v>7684</v>
@@ -79961,47 +79976,47 @@
         <v>7713</v>
       </c>
       <c r="G55" t="s">
-        <v>7820</v>
+        <v>7661</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>7639</v>
+        <v>7819</v>
       </c>
       <c r="B56" t="s">
-        <v>7685</v>
+        <v>7684</v>
       </c>
       <c r="C56" t="s">
         <v>7660</v>
       </c>
       <c r="D56" t="s">
-        <v>7645</v>
+        <v>7644</v>
       </c>
       <c r="E56" t="s">
-        <v>7652</v>
+        <v>7651</v>
       </c>
       <c r="F56" t="s">
         <v>7713</v>
       </c>
       <c r="G56" t="s">
-        <v>7661</v>
+        <v>7820</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>7640</v>
+        <v>7639</v>
       </c>
       <c r="B57" t="s">
-        <v>7686</v>
+        <v>7685</v>
       </c>
       <c r="C57" t="s">
         <v>7660</v>
       </c>
       <c r="D57" t="s">
-        <v>7646</v>
+        <v>7645</v>
       </c>
       <c r="E57" t="s">
-        <v>7653</v>
+        <v>7652</v>
       </c>
       <c r="F57" t="s">
         <v>7713</v>
@@ -80012,19 +80027,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>7641</v>
+        <v>7640</v>
       </c>
       <c r="B58" t="s">
-        <v>7687</v>
+        <v>7686</v>
       </c>
       <c r="C58" t="s">
         <v>7660</v>
       </c>
       <c r="D58" t="s">
-        <v>7647</v>
+        <v>7646</v>
       </c>
       <c r="E58" t="s">
-        <v>7654</v>
+        <v>7653</v>
       </c>
       <c r="F58" t="s">
         <v>7713</v>
@@ -80035,19 +80050,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>7642</v>
+        <v>7641</v>
       </c>
       <c r="B59" t="s">
-        <v>7688</v>
+        <v>7687</v>
       </c>
       <c r="C59" t="s">
         <v>7660</v>
       </c>
       <c r="D59" t="s">
-        <v>7648</v>
+        <v>7647</v>
       </c>
       <c r="E59" t="s">
-        <v>7655</v>
+        <v>7654</v>
       </c>
       <c r="F59" t="s">
         <v>7713</v>
@@ -80058,19 +80073,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>7643</v>
+        <v>7642</v>
       </c>
       <c r="B60" t="s">
-        <v>7689</v>
+        <v>7688</v>
       </c>
       <c r="C60" t="s">
         <v>7660</v>
       </c>
       <c r="D60" t="s">
-        <v>7649</v>
+        <v>7648</v>
       </c>
       <c r="E60" t="s">
-        <v>7656</v>
+        <v>7655</v>
       </c>
       <c r="F60" t="s">
         <v>7713</v>
@@ -80081,42 +80096,42 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>7662</v>
+        <v>7643</v>
       </c>
       <c r="B61" t="s">
-        <v>7690</v>
+        <v>7689</v>
       </c>
       <c r="C61" t="s">
-        <v>7674</v>
+        <v>7660</v>
       </c>
       <c r="D61" t="s">
-        <v>7668</v>
+        <v>7649</v>
       </c>
       <c r="E61" t="s">
-        <v>7675</v>
+        <v>7656</v>
       </c>
       <c r="F61" t="s">
         <v>7713</v>
       </c>
       <c r="G61" t="s">
-        <v>7681</v>
+        <v>7661</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>7663</v>
+        <v>7662</v>
       </c>
       <c r="B62" t="s">
-        <v>7691</v>
+        <v>7690</v>
       </c>
       <c r="C62" t="s">
         <v>7674</v>
       </c>
       <c r="D62" t="s">
-        <v>7669</v>
+        <v>7668</v>
       </c>
       <c r="E62" t="s">
-        <v>7676</v>
+        <v>7675</v>
       </c>
       <c r="F62" t="s">
         <v>7713</v>
@@ -80127,19 +80142,19 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>7664</v>
+        <v>7663</v>
       </c>
       <c r="B63" t="s">
-        <v>7692</v>
+        <v>7691</v>
       </c>
       <c r="C63" t="s">
         <v>7674</v>
       </c>
       <c r="D63" t="s">
-        <v>7670</v>
+        <v>7669</v>
       </c>
       <c r="E63" t="s">
-        <v>7677</v>
+        <v>7676</v>
       </c>
       <c r="F63" t="s">
         <v>7713</v>
@@ -80150,19 +80165,19 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>7665</v>
+        <v>7664</v>
       </c>
       <c r="B64" t="s">
-        <v>7693</v>
+        <v>7692</v>
       </c>
       <c r="C64" t="s">
         <v>7674</v>
       </c>
       <c r="D64" t="s">
-        <v>7671</v>
+        <v>7670</v>
       </c>
       <c r="E64" t="s">
-        <v>7678</v>
+        <v>7677</v>
       </c>
       <c r="F64" t="s">
         <v>7713</v>
@@ -80173,19 +80188,19 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>7666</v>
+        <v>7665</v>
       </c>
       <c r="B65" t="s">
-        <v>7694</v>
+        <v>7693</v>
       </c>
       <c r="C65" t="s">
         <v>7674</v>
       </c>
       <c r="D65" t="s">
-        <v>7672</v>
+        <v>7671</v>
       </c>
       <c r="E65" t="s">
-        <v>7679</v>
+        <v>7678</v>
       </c>
       <c r="F65" t="s">
         <v>7713</v>
@@ -80196,22 +80211,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>7667</v>
+        <v>7666</v>
       </c>
       <c r="B66" t="s">
-        <v>7695</v>
+        <v>7694</v>
       </c>
       <c r="C66" t="s">
         <v>7674</v>
       </c>
       <c r="D66" t="s">
-        <v>7673</v>
+        <v>7672</v>
       </c>
       <c r="E66" t="s">
-        <v>7680</v>
+        <v>7679</v>
       </c>
       <c r="F66" t="s">
-        <v>7421</v>
+        <v>7713</v>
       </c>
       <c r="G66" t="s">
         <v>7681</v>
@@ -80219,180 +80234,180 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>7511</v>
+        <v>7667</v>
       </c>
       <c r="B67" t="s">
-        <v>7619</v>
+        <v>7695</v>
       </c>
       <c r="C67" t="s">
-        <v>7513</v>
+        <v>7674</v>
       </c>
       <c r="D67" t="s">
-        <v>7619</v>
+        <v>7673</v>
       </c>
       <c r="E67" t="s">
-        <v>7620</v>
+        <v>7680</v>
       </c>
       <c r="F67" t="s">
-        <v>7634</v>
+        <v>7421</v>
       </c>
       <c r="G67" t="s">
-        <v>7621</v>
+        <v>7681</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>7515</v>
+        <v>7511</v>
       </c>
       <c r="B68" t="s">
-        <v>7514</v>
+        <v>7619</v>
       </c>
       <c r="C68" t="s">
         <v>7513</v>
       </c>
       <c r="D68" t="s">
-        <v>7514</v>
+        <v>7619</v>
       </c>
       <c r="E68" t="s">
-        <v>7518</v>
+        <v>7620</v>
       </c>
       <c r="F68" t="s">
         <v>7634</v>
       </c>
       <c r="G68" t="s">
-        <v>7814</v>
+        <v>7621</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>7516</v>
+        <v>7515</v>
       </c>
       <c r="B69" t="s">
-        <v>7512</v>
+        <v>7514</v>
       </c>
       <c r="C69" t="s">
         <v>7513</v>
       </c>
       <c r="D69" t="s">
-        <v>7512</v>
+        <v>7514</v>
       </c>
       <c r="E69" t="s">
-        <v>7520</v>
+        <v>7518</v>
       </c>
       <c r="F69" t="s">
         <v>7634</v>
       </c>
       <c r="G69" t="s">
-        <v>7815</v>
+        <v>7814</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>7521</v>
+        <v>7516</v>
       </c>
       <c r="B70" t="s">
-        <v>7517</v>
+        <v>7512</v>
       </c>
       <c r="C70" t="s">
         <v>7513</v>
       </c>
       <c r="D70" t="s">
-        <v>7517</v>
+        <v>7512</v>
       </c>
       <c r="E70" t="s">
-        <v>7519</v>
+        <v>7520</v>
       </c>
       <c r="F70" t="s">
         <v>7634</v>
       </c>
       <c r="G70" t="s">
-        <v>7816</v>
+        <v>7815</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>7524</v>
+        <v>7521</v>
       </c>
       <c r="B71" t="s">
-        <v>7522</v>
+        <v>7517</v>
       </c>
       <c r="C71" t="s">
         <v>7513</v>
       </c>
       <c r="D71" t="s">
-        <v>7522</v>
+        <v>7517</v>
       </c>
       <c r="E71" t="s">
-        <v>7523</v>
+        <v>7519</v>
       </c>
       <c r="F71" t="s">
         <v>7634</v>
       </c>
       <c r="G71" t="s">
-        <v>7817</v>
+        <v>7816</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>7618</v>
+        <v>7524</v>
       </c>
       <c r="B72" t="s">
-        <v>7525</v>
+        <v>7522</v>
       </c>
       <c r="C72" t="s">
         <v>7513</v>
       </c>
       <c r="D72" t="s">
-        <v>7525</v>
+        <v>7522</v>
       </c>
       <c r="E72" t="s">
-        <v>7526</v>
+        <v>7523</v>
       </c>
       <c r="F72" t="s">
         <v>7634</v>
       </c>
       <c r="G72" t="s">
-        <v>7818</v>
+        <v>7817</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>7708</v>
+        <v>7618</v>
       </c>
       <c r="B73" t="s">
-        <v>7709</v>
+        <v>7525</v>
       </c>
       <c r="C73" t="s">
-        <v>7710</v>
+        <v>7513</v>
       </c>
       <c r="D73" t="s">
-        <v>7711</v>
+        <v>7525</v>
       </c>
       <c r="E73" t="s">
-        <v>7712</v>
+        <v>7526</v>
       </c>
       <c r="F73" t="s">
-        <v>7713</v>
+        <v>7634</v>
       </c>
       <c r="G73" t="s">
-        <v>7714</v>
+        <v>7818</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>7724</v>
+        <v>7708</v>
       </c>
       <c r="B74" t="s">
-        <v>7715</v>
+        <v>7709</v>
       </c>
       <c r="C74" t="s">
         <v>7710</v>
       </c>
       <c r="D74" t="s">
-        <v>7733</v>
+        <v>7711</v>
       </c>
       <c r="E74" t="s">
-        <v>7736</v>
+        <v>7712</v>
       </c>
       <c r="F74" t="s">
         <v>7713</v>
@@ -80403,19 +80418,19 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>7725</v>
+        <v>7724</v>
       </c>
       <c r="B75" t="s">
-        <v>7716</v>
+        <v>7715</v>
       </c>
       <c r="C75" t="s">
         <v>7710</v>
       </c>
       <c r="D75" t="s">
-        <v>7734</v>
+        <v>7733</v>
       </c>
       <c r="E75" t="s">
-        <v>7737</v>
+        <v>7736</v>
       </c>
       <c r="F75" t="s">
         <v>7713</v>
@@ -80426,19 +80441,19 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>7726</v>
+        <v>7725</v>
       </c>
       <c r="B76" t="s">
-        <v>7717</v>
+        <v>7716</v>
       </c>
       <c r="C76" t="s">
         <v>7710</v>
       </c>
       <c r="D76" t="s">
-        <v>7735</v>
+        <v>7734</v>
       </c>
       <c r="E76" t="s">
-        <v>7738</v>
+        <v>7737</v>
       </c>
       <c r="F76" t="s">
         <v>7713</v>
@@ -80449,19 +80464,19 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>7727</v>
+        <v>7726</v>
       </c>
       <c r="B77" t="s">
-        <v>7718</v>
+        <v>7717</v>
       </c>
       <c r="C77" t="s">
         <v>7710</v>
       </c>
       <c r="D77" t="s">
-        <v>7800</v>
+        <v>7735</v>
       </c>
       <c r="E77" t="s">
-        <v>7739</v>
+        <v>7738</v>
       </c>
       <c r="F77" t="s">
         <v>7713</v>
@@ -80472,19 +80487,19 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>7728</v>
+        <v>7727</v>
       </c>
       <c r="B78" t="s">
-        <v>7719</v>
+        <v>7718</v>
       </c>
       <c r="C78" t="s">
         <v>7710</v>
       </c>
       <c r="D78" t="s">
-        <v>7801</v>
+        <v>7800</v>
       </c>
       <c r="E78" t="s">
-        <v>7740</v>
+        <v>7739</v>
       </c>
       <c r="F78" t="s">
         <v>7713</v>
@@ -80495,19 +80510,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>7729</v>
+        <v>7728</v>
       </c>
       <c r="B79" t="s">
-        <v>7720</v>
+        <v>7719</v>
       </c>
       <c r="C79" t="s">
         <v>7710</v>
       </c>
       <c r="D79" t="s">
-        <v>7802</v>
+        <v>7801</v>
       </c>
       <c r="E79" t="s">
-        <v>7741</v>
+        <v>7740</v>
       </c>
       <c r="F79" t="s">
         <v>7713</v>
@@ -80518,19 +80533,19 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>7730</v>
+        <v>7729</v>
       </c>
       <c r="B80" t="s">
-        <v>7721</v>
+        <v>7720</v>
       </c>
       <c r="C80" t="s">
         <v>7710</v>
       </c>
       <c r="D80" t="s">
-        <v>7803</v>
+        <v>7802</v>
       </c>
       <c r="E80" t="s">
-        <v>7742</v>
+        <v>7741</v>
       </c>
       <c r="F80" t="s">
         <v>7713</v>
@@ -80541,19 +80556,19 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>7731</v>
+        <v>7730</v>
       </c>
       <c r="B81" t="s">
-        <v>7722</v>
+        <v>7721</v>
       </c>
       <c r="C81" t="s">
         <v>7710</v>
       </c>
       <c r="D81" t="s">
-        <v>7804</v>
+        <v>7803</v>
       </c>
       <c r="E81" t="s">
-        <v>7743</v>
+        <v>7742</v>
       </c>
       <c r="F81" t="s">
         <v>7713</v>
@@ -80564,19 +80579,19 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>7732</v>
+        <v>7731</v>
       </c>
       <c r="B82" t="s">
-        <v>7723</v>
+        <v>7722</v>
       </c>
       <c r="C82" t="s">
         <v>7710</v>
       </c>
       <c r="D82" t="s">
-        <v>7805</v>
+        <v>7804</v>
       </c>
       <c r="E82" t="s">
-        <v>7744</v>
+        <v>7743</v>
       </c>
       <c r="F82" t="s">
         <v>7713</v>
@@ -80587,22 +80602,22 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>7784</v>
+        <v>7732</v>
       </c>
       <c r="B83" t="s">
-        <v>7709</v>
+        <v>7723</v>
       </c>
       <c r="C83" t="s">
-        <v>7751</v>
+        <v>7710</v>
       </c>
       <c r="D83" t="s">
-        <v>7792</v>
+        <v>7805</v>
       </c>
       <c r="E83" t="s">
-        <v>7806</v>
+        <v>7744</v>
       </c>
       <c r="F83" t="s">
-        <v>6374</v>
+        <v>7713</v>
       </c>
       <c r="G83" t="s">
         <v>7714</v>
@@ -80610,19 +80625,19 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>7785</v>
+        <v>7784</v>
       </c>
       <c r="B84" t="s">
-        <v>7717</v>
+        <v>7709</v>
       </c>
       <c r="C84" t="s">
         <v>7751</v>
       </c>
       <c r="D84" t="s">
-        <v>7793</v>
+        <v>7792</v>
       </c>
       <c r="E84" t="s">
-        <v>7807</v>
+        <v>7806</v>
       </c>
       <c r="F84" t="s">
         <v>6374</v>
@@ -80633,19 +80648,19 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>7786</v>
+        <v>7785</v>
       </c>
       <c r="B85" t="s">
-        <v>7718</v>
+        <v>7717</v>
       </c>
       <c r="C85" t="s">
         <v>7751</v>
       </c>
       <c r="D85" t="s">
-        <v>7794</v>
+        <v>7793</v>
       </c>
       <c r="E85" t="s">
-        <v>7808</v>
+        <v>7807</v>
       </c>
       <c r="F85" t="s">
         <v>6374</v>
@@ -80656,19 +80671,19 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>7787</v>
+        <v>7786</v>
       </c>
       <c r="B86" t="s">
-        <v>7719</v>
+        <v>7718</v>
       </c>
       <c r="C86" t="s">
         <v>7751</v>
       </c>
       <c r="D86" t="s">
-        <v>7795</v>
+        <v>7794</v>
       </c>
       <c r="E86" t="s">
-        <v>7809</v>
+        <v>7808</v>
       </c>
       <c r="F86" t="s">
         <v>6374</v>
@@ -80679,19 +80694,19 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>7788</v>
+        <v>7787</v>
       </c>
       <c r="B87" t="s">
-        <v>7720</v>
+        <v>7719</v>
       </c>
       <c r="C87" t="s">
         <v>7751</v>
       </c>
       <c r="D87" t="s">
-        <v>7796</v>
+        <v>7795</v>
       </c>
       <c r="E87" t="s">
-        <v>7810</v>
+        <v>7809</v>
       </c>
       <c r="F87" t="s">
         <v>6374</v>
@@ -80702,19 +80717,19 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>7789</v>
+        <v>7788</v>
       </c>
       <c r="B88" t="s">
-        <v>7721</v>
+        <v>7720</v>
       </c>
       <c r="C88" t="s">
         <v>7751</v>
       </c>
       <c r="D88" t="s">
-        <v>7797</v>
+        <v>7796</v>
       </c>
       <c r="E88" t="s">
-        <v>7811</v>
+        <v>7810</v>
       </c>
       <c r="F88" t="s">
         <v>6374</v>
@@ -80725,19 +80740,19 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>7790</v>
+        <v>7789</v>
       </c>
       <c r="B89" t="s">
-        <v>7722</v>
+        <v>7721</v>
       </c>
       <c r="C89" t="s">
         <v>7751</v>
       </c>
       <c r="D89" t="s">
-        <v>7798</v>
+        <v>7797</v>
       </c>
       <c r="E89" t="s">
-        <v>7812</v>
+        <v>7811</v>
       </c>
       <c r="F89" t="s">
         <v>6374</v>
@@ -80748,19 +80763,19 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>7791</v>
+        <v>7790</v>
       </c>
       <c r="B90" t="s">
-        <v>7723</v>
+        <v>7722</v>
       </c>
       <c r="C90" t="s">
         <v>7751</v>
       </c>
       <c r="D90" t="s">
-        <v>7799</v>
+        <v>7798</v>
       </c>
       <c r="E90" t="s">
-        <v>7813</v>
+        <v>7812</v>
       </c>
       <c r="F90" t="s">
         <v>6374</v>
@@ -80771,240 +80786,240 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>7630</v>
+        <v>7791</v>
       </c>
       <c r="B91" t="s">
-        <v>7631</v>
+        <v>7723</v>
       </c>
       <c r="C91" t="s">
-        <v>7632</v>
+        <v>7751</v>
       </c>
       <c r="D91" t="s">
-        <v>7631</v>
+        <v>7799</v>
       </c>
       <c r="E91" t="s">
-        <v>7633</v>
+        <v>7813</v>
       </c>
       <c r="F91" t="s">
-        <v>7634</v>
+        <v>6374</v>
       </c>
       <c r="G91" t="s">
-        <v>7635</v>
+        <v>7714</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>6439</v>
+        <v>7630</v>
       </c>
       <c r="B92" t="s">
-        <v>6442</v>
+        <v>7631</v>
       </c>
       <c r="C92" t="s">
-        <v>6440</v>
+        <v>7632</v>
       </c>
       <c r="D92" t="s">
-        <v>6441</v>
+        <v>7631</v>
       </c>
       <c r="E92" t="s">
-        <v>6447</v>
+        <v>7633</v>
       </c>
       <c r="F92" t="s">
-        <v>6443</v>
+        <v>7634</v>
       </c>
       <c r="G92" t="s">
-        <v>7657</v>
+        <v>7635</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>6468</v>
+        <v>6439</v>
       </c>
       <c r="B93" t="s">
-        <v>6469</v>
+        <v>6442</v>
       </c>
       <c r="C93" t="s">
-        <v>6470</v>
+        <v>6440</v>
       </c>
       <c r="D93" t="s">
-        <v>6471</v>
+        <v>6441</v>
       </c>
       <c r="E93" t="s">
-        <v>6472</v>
+        <v>6447</v>
       </c>
       <c r="F93" t="s">
         <v>6443</v>
       </c>
       <c r="G93" t="s">
-        <v>7658</v>
+        <v>7657</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>6473</v>
+        <v>6468</v>
       </c>
       <c r="B94" t="s">
-        <v>6475</v>
+        <v>6469</v>
       </c>
       <c r="C94" t="s">
-        <v>6440</v>
+        <v>6470</v>
       </c>
       <c r="D94" t="s">
-        <v>6474</v>
+        <v>6471</v>
       </c>
       <c r="E94" t="s">
-        <v>6476</v>
+        <v>6472</v>
       </c>
       <c r="F94" t="s">
         <v>6443</v>
       </c>
       <c r="G94" t="s">
-        <v>7659</v>
+        <v>7658</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>6420</v>
+        <v>6473</v>
       </c>
       <c r="B95" t="s">
-        <v>6453</v>
+        <v>6475</v>
       </c>
       <c r="C95" t="s">
-        <v>6421</v>
+        <v>6440</v>
       </c>
       <c r="D95" t="s">
-        <v>6422</v>
+        <v>6474</v>
       </c>
       <c r="E95" t="s">
-        <v>6444</v>
+        <v>6476</v>
       </c>
       <c r="F95" t="s">
-        <v>6423</v>
+        <v>6443</v>
       </c>
       <c r="G95" t="s">
-        <v>6428</v>
+        <v>7659</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>6424</v>
+        <v>6420</v>
       </c>
       <c r="B96" t="s">
-        <v>6454</v>
+        <v>6453</v>
       </c>
       <c r="C96" t="s">
-        <v>6425</v>
+        <v>6421</v>
       </c>
       <c r="D96" t="s">
-        <v>6426</v>
+        <v>6422</v>
       </c>
       <c r="E96" t="s">
-        <v>6445</v>
+        <v>6444</v>
       </c>
       <c r="F96" t="s">
         <v>6423</v>
       </c>
       <c r="G96" t="s">
-        <v>6427</v>
+        <v>6428</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>6431</v>
+        <v>6424</v>
       </c>
       <c r="B97" t="s">
-        <v>6452</v>
+        <v>6454</v>
       </c>
       <c r="C97" t="s">
-        <v>6430</v>
+        <v>6425</v>
       </c>
       <c r="D97" t="s">
-        <v>6434</v>
+        <v>6426</v>
       </c>
       <c r="E97" t="s">
-        <v>6446</v>
+        <v>6445</v>
       </c>
       <c r="F97" t="s">
         <v>6423</v>
       </c>
       <c r="G97" t="s">
-        <v>6429</v>
+        <v>6427</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>6448</v>
+        <v>6431</v>
       </c>
       <c r="B98" t="s">
-        <v>6433</v>
+        <v>6452</v>
       </c>
       <c r="C98" t="s">
-        <v>6432</v>
+        <v>6430</v>
       </c>
       <c r="D98" t="s">
-        <v>6433</v>
+        <v>6434</v>
       </c>
       <c r="E98" t="s">
-        <v>6450</v>
+        <v>6446</v>
       </c>
       <c r="F98" t="s">
         <v>6423</v>
       </c>
       <c r="G98" t="s">
-        <v>6435</v>
+        <v>6429</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>7426</v>
+        <v>6448</v>
       </c>
       <c r="B99" t="s">
-        <v>6451</v>
+        <v>6433</v>
       </c>
       <c r="C99" t="s">
-        <v>6436</v>
+        <v>6432</v>
       </c>
       <c r="D99" t="s">
-        <v>6437</v>
+        <v>6433</v>
       </c>
       <c r="E99" t="s">
-        <v>6449</v>
+        <v>6450</v>
       </c>
       <c r="F99" t="s">
         <v>6423</v>
       </c>
       <c r="G99" t="s">
-        <v>6438</v>
+        <v>6435</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>7427</v>
+        <v>7426</v>
       </c>
       <c r="B100" t="s">
-        <v>7428</v>
+        <v>6451</v>
       </c>
       <c r="C100" t="s">
-        <v>7429</v>
-      </c>
-      <c r="D100">
-        <v>1085</v>
+        <v>6436</v>
+      </c>
+      <c r="D100" t="s">
+        <v>6437</v>
       </c>
       <c r="E100" t="s">
-        <v>7430</v>
+        <v>6449</v>
       </c>
       <c r="F100" t="s">
         <v>6423</v>
       </c>
       <c r="G100" t="s">
-        <v>7494</v>
+        <v>6438</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>7431</v>
+        <v>7427</v>
       </c>
       <c r="B101" t="s">
-        <v>7706</v>
+        <v>7428</v>
       </c>
       <c r="C101" t="s">
         <v>7429</v>
@@ -81013,44 +81028,44 @@
         <v>1085</v>
       </c>
       <c r="E101" t="s">
-        <v>7491</v>
+        <v>7430</v>
       </c>
       <c r="F101" t="s">
         <v>6423</v>
       </c>
       <c r="G101" t="s">
-        <v>7495</v>
+        <v>7494</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>7487</v>
+        <v>7431</v>
       </c>
       <c r="B102" t="s">
-        <v>7488</v>
+        <v>7706</v>
       </c>
       <c r="C102" t="s">
         <v>7429</v>
       </c>
       <c r="D102">
-        <v>1164</v>
+        <v>1085</v>
       </c>
       <c r="E102" t="s">
-        <v>7489</v>
+        <v>7491</v>
       </c>
       <c r="F102" t="s">
         <v>6423</v>
       </c>
       <c r="G102" t="s">
-        <v>7496</v>
+        <v>7495</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>7490</v>
+        <v>7487</v>
       </c>
       <c r="B103" t="s">
-        <v>7704</v>
+        <v>7488</v>
       </c>
       <c r="C103" t="s">
         <v>7429</v>
@@ -81059,21 +81074,21 @@
         <v>1164</v>
       </c>
       <c r="E103" t="s">
-        <v>7492</v>
+        <v>7489</v>
       </c>
       <c r="F103" t="s">
         <v>6423</v>
       </c>
       <c r="G103" t="s">
-        <v>7493</v>
+        <v>7496</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>7700</v>
+        <v>7490</v>
       </c>
       <c r="B104" t="s">
-        <v>7701</v>
+        <v>7704</v>
       </c>
       <c r="C104" t="s">
         <v>7429</v>
@@ -81082,44 +81097,44 @@
         <v>1164</v>
       </c>
       <c r="E104" t="s">
-        <v>7702</v>
+        <v>7492</v>
       </c>
       <c r="F104" t="s">
         <v>6423</v>
       </c>
       <c r="G104" t="s">
-        <v>7707</v>
+        <v>7493</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>7497</v>
+        <v>7700</v>
       </c>
       <c r="B105" t="s">
-        <v>7498</v>
+        <v>7701</v>
       </c>
       <c r="C105" t="s">
         <v>7429</v>
       </c>
       <c r="D105">
-        <v>3328</v>
+        <v>1164</v>
       </c>
       <c r="E105" t="s">
-        <v>7499</v>
+        <v>7702</v>
       </c>
       <c r="F105" t="s">
         <v>6423</v>
       </c>
       <c r="G105" t="s">
-        <v>7500</v>
+        <v>7707</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>7503</v>
+        <v>7497</v>
       </c>
       <c r="B106" t="s">
-        <v>7703</v>
+        <v>7498</v>
       </c>
       <c r="C106" t="s">
         <v>7429</v>
@@ -81128,21 +81143,21 @@
         <v>3328</v>
       </c>
       <c r="E106" t="s">
-        <v>7502</v>
+        <v>7499</v>
       </c>
       <c r="F106" t="s">
         <v>6423</v>
       </c>
       <c r="G106" t="s">
-        <v>7501</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>7696</v>
+        <v>7503</v>
       </c>
       <c r="B107" t="s">
-        <v>7699</v>
+        <v>7703</v>
       </c>
       <c r="C107" t="s">
         <v>7429</v>
@@ -81151,44 +81166,44 @@
         <v>3328</v>
       </c>
       <c r="E107" t="s">
-        <v>7697</v>
+        <v>7502</v>
       </c>
       <c r="F107" t="s">
         <v>6423</v>
       </c>
       <c r="G107" t="s">
-        <v>7698</v>
+        <v>7501</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>7504</v>
+        <v>7696</v>
       </c>
       <c r="B108" t="s">
-        <v>7506</v>
+        <v>7699</v>
       </c>
       <c r="C108" t="s">
         <v>7429</v>
       </c>
       <c r="D108">
-        <v>815</v>
+        <v>3328</v>
       </c>
       <c r="E108" t="s">
-        <v>7507</v>
+        <v>7697</v>
       </c>
       <c r="F108" t="s">
         <v>6423</v>
       </c>
       <c r="G108" t="s">
-        <v>7505</v>
+        <v>7698</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>7510</v>
+        <v>7504</v>
       </c>
       <c r="B109" t="s">
-        <v>7705</v>
+        <v>7506</v>
       </c>
       <c r="C109" t="s">
         <v>7429</v>
@@ -81197,73 +81212,76 @@
         <v>815</v>
       </c>
       <c r="E109" t="s">
-        <v>7509</v>
+        <v>7507</v>
       </c>
       <c r="F109" t="s">
         <v>6423</v>
       </c>
       <c r="G109" t="s">
-        <v>7508</v>
+        <v>7505</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>7821</v>
+        <v>7510</v>
       </c>
       <c r="B110" t="s">
-        <v>7822</v>
+        <v>7705</v>
       </c>
       <c r="C110" t="s">
-        <v>7823</v>
-      </c>
-      <c r="D110" t="s">
-        <v>7824</v>
+        <v>7429</v>
+      </c>
+      <c r="D110">
+        <v>815</v>
       </c>
       <c r="E110" t="s">
-        <v>7825</v>
+        <v>7509</v>
       </c>
       <c r="F110" t="s">
-        <v>7713</v>
+        <v>6423</v>
       </c>
       <c r="G110" t="s">
-        <v>7423</v>
+        <v>7508</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>7829</v>
+        <v>7821</v>
       </c>
       <c r="B111" t="s">
-        <v>7830</v>
+        <v>7822</v>
       </c>
       <c r="C111" t="s">
-        <v>6373</v>
-      </c>
-      <c r="D111">
-        <v>1704853</v>
+        <v>7823</v>
+      </c>
+      <c r="D111" t="s">
+        <v>7824</v>
       </c>
       <c r="E111" t="s">
-        <v>7831</v>
+        <v>7825</v>
       </c>
       <c r="F111" t="s">
-        <v>6374</v>
+        <v>7713</v>
+      </c>
+      <c r="G111" t="s">
+        <v>7423</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>7832</v>
+        <v>7829</v>
       </c>
       <c r="B112" t="s">
-        <v>7833</v>
+        <v>7830</v>
       </c>
       <c r="C112" t="s">
         <v>6373</v>
       </c>
       <c r="D112">
-        <v>1704854</v>
+        <v>1704853</v>
       </c>
       <c r="E112" t="s">
-        <v>7842</v>
+        <v>7831</v>
       </c>
       <c r="F112" t="s">
         <v>6374</v>
@@ -81271,19 +81289,19 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>7834</v>
+        <v>7832</v>
       </c>
       <c r="B113" t="s">
-        <v>7835</v>
+        <v>7833</v>
       </c>
       <c r="C113" t="s">
         <v>6373</v>
       </c>
       <c r="D113">
-        <v>1704857</v>
+        <v>1704854</v>
       </c>
       <c r="E113" t="s">
-        <v>7843</v>
+        <v>7842</v>
       </c>
       <c r="F113" t="s">
         <v>6374</v>
@@ -81291,19 +81309,19 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>7827</v>
+        <v>7834</v>
       </c>
       <c r="B114" t="s">
-        <v>7826</v>
+        <v>7835</v>
       </c>
       <c r="C114" t="s">
         <v>6373</v>
       </c>
       <c r="D114">
-        <v>1704858</v>
+        <v>1704857</v>
       </c>
       <c r="E114" t="s">
-        <v>7828</v>
+        <v>7843</v>
       </c>
       <c r="F114" t="s">
         <v>6374</v>
@@ -81311,19 +81329,19 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>7836</v>
+        <v>7827</v>
       </c>
       <c r="B115" t="s">
-        <v>7837</v>
+        <v>7826</v>
       </c>
       <c r="C115" t="s">
         <v>6373</v>
       </c>
       <c r="D115">
-        <v>1704859</v>
+        <v>1704858</v>
       </c>
       <c r="E115" t="s">
-        <v>7844</v>
+        <v>7828</v>
       </c>
       <c r="F115" t="s">
         <v>6374</v>
@@ -81331,19 +81349,19 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>7838</v>
+        <v>7836</v>
       </c>
       <c r="B116" t="s">
-        <v>7839</v>
+        <v>7837</v>
       </c>
       <c r="C116" t="s">
         <v>6373</v>
       </c>
       <c r="D116">
-        <v>1704860</v>
+        <v>1704859</v>
       </c>
       <c r="E116" t="s">
-        <v>7845</v>
+        <v>7844</v>
       </c>
       <c r="F116" t="s">
         <v>6374</v>
@@ -81351,32 +81369,52 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>7840</v>
+        <v>7838</v>
       </c>
       <c r="B117" t="s">
-        <v>7841</v>
+        <v>7839</v>
       </c>
       <c r="C117" t="s">
         <v>6373</v>
       </c>
       <c r="D117">
-        <v>1704861</v>
+        <v>1704860</v>
       </c>
       <c r="E117" t="s">
-        <v>7846</v>
+        <v>7845</v>
       </c>
       <c r="F117" t="s">
         <v>6374</v>
       </c>
     </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>7840</v>
+      </c>
+      <c r="B118" t="s">
+        <v>7841</v>
+      </c>
+      <c r="C118" t="s">
+        <v>6373</v>
+      </c>
+      <c r="D118">
+        <v>1704861</v>
+      </c>
+      <c r="E118" t="s">
+        <v>7846</v>
+      </c>
+      <c r="F118" t="s">
+        <v>6374</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G29">
-    <sortState ref="A2:G110">
+    <sortState ref="A2:G111">
       <sortCondition ref="A1:A29"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A111:F118">
-    <sortCondition ref="A111"/>
+  <sortState ref="A112:F119">
+    <sortCondition ref="A112"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>